<commit_message>
"Monte Alto added to MM347"
</commit_message>
<xml_diff>
--- a/trackedvessels.xlsx
+++ b/trackedvessels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/Vesseltimeline/VesselTimeline_dataGet-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="143" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D23AFB5D-ED1C-4609-96B2-B7A778BCEFA5}"/>
+  <xr:revisionPtr revIDLastSave="149" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A24BFF1-5C75-41B9-827F-ED0F7983FF93}"/>
   <bookViews>
-    <workbookView xWindow="25510" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="51420" windowHeight="13900" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="266">
   <si>
     <t>Santa Rosa</t>
   </si>
@@ -828,6 +828,12 @@
   </si>
   <si>
     <t>Monte Sarmiento</t>
+  </si>
+  <si>
+    <t>Monte Alto</t>
+  </si>
+  <si>
+    <t>Monte</t>
   </si>
 </sst>
 </file>
@@ -1185,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A49309-98C8-6143-85DD-C6C0E46E1D27}">
-  <dimension ref="A1:D225"/>
+  <dimension ref="A1:D226"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1424,13 +1430,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>250</v>
+        <v>264</v>
       </c>
       <c r="B17">
-        <v>9299939</v>
+        <v>9283227</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>265</v>
       </c>
       <c r="D17" t="s">
         <v>62</v>
@@ -1438,13 +1444,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>250</v>
       </c>
       <c r="B18">
-        <v>9303522</v>
+        <v>9299939</v>
       </c>
       <c r="C18" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
         <v>62</v>
@@ -1452,10 +1458,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>251</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>9303534</v>
+        <v>9303522</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
@@ -1466,10 +1472,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>251</v>
       </c>
       <c r="B20">
-        <v>9306550</v>
+        <v>9303534</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
@@ -1480,13 +1486,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B21">
-        <v>9699189</v>
+        <v>9306550</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>62</v>
@@ -1494,10 +1500,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22">
-        <v>9699191</v>
+        <v>9699189</v>
       </c>
       <c r="C22" t="s">
         <v>53</v>
@@ -1508,10 +1514,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23">
-        <v>9699206</v>
+        <v>9699191</v>
       </c>
       <c r="C23" t="s">
         <v>53</v>
@@ -1522,13 +1528,13 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B24">
-        <v>9430387</v>
+        <v>9699206</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
         <v>62</v>
@@ -1536,10 +1542,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B25">
-        <v>9430399</v>
+        <v>9430387</v>
       </c>
       <c r="C25" t="s">
         <v>61</v>
@@ -1550,10 +1556,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>9444845</v>
+        <v>9430399</v>
       </c>
       <c r="C26" t="s">
         <v>61</v>
@@ -1564,10 +1570,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27">
-        <v>9444716</v>
+        <v>9444845</v>
       </c>
       <c r="C27" t="s">
         <v>61</v>
@@ -1578,10 +1584,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>252</v>
+        <v>16</v>
       </c>
       <c r="B28">
-        <v>9444728</v>
+        <v>9444716</v>
       </c>
       <c r="C28" t="s">
         <v>61</v>
@@ -1592,10 +1598,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>17</v>
+        <v>252</v>
       </c>
       <c r="B29">
-        <v>9444730</v>
+        <v>9444728</v>
       </c>
       <c r="C29" t="s">
         <v>61</v>
@@ -1606,10 +1612,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30">
-        <v>9444742</v>
+        <v>9444730</v>
       </c>
       <c r="C30" t="s">
         <v>61</v>
@@ -1620,10 +1626,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>253</v>
+        <v>18</v>
       </c>
       <c r="B31">
-        <v>9425382</v>
+        <v>9444742</v>
       </c>
       <c r="C31" t="s">
         <v>61</v>
@@ -1634,10 +1640,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>0</v>
+        <v>253</v>
       </c>
       <c r="B32">
-        <v>9430363</v>
+        <v>9425382</v>
       </c>
       <c r="C32" t="s">
         <v>61</v>
@@ -1648,10 +1654,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B33">
-        <v>9430375</v>
+        <v>9430363</v>
       </c>
       <c r="C33" t="s">
         <v>61</v>
@@ -1662,13 +1668,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B34">
-        <v>9348053</v>
+        <v>9430375</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
         <v>62</v>
@@ -1676,10 +1682,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B35">
-        <v>9348065</v>
+        <v>9348053</v>
       </c>
       <c r="C35" t="s">
         <v>54</v>
@@ -1690,10 +1696,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B36">
-        <v>9348077</v>
+        <v>9348065</v>
       </c>
       <c r="C36" t="s">
         <v>54</v>
@@ -1704,13 +1710,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B37">
-        <v>9283186</v>
+        <v>9348077</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
         <v>62</v>
@@ -1718,10 +1724,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B38">
-        <v>9283198</v>
+        <v>9283186</v>
       </c>
       <c r="C38" t="s">
         <v>55</v>
@@ -1732,10 +1738,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39">
-        <v>9283203</v>
+        <v>9283198</v>
       </c>
       <c r="C39" t="s">
         <v>55</v>
@@ -1746,10 +1752,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B40">
-        <v>9283215</v>
+        <v>9283203</v>
       </c>
       <c r="C40" t="s">
         <v>55</v>
@@ -1760,10 +1766,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41">
-        <v>9283239</v>
+        <v>9283215</v>
       </c>
       <c r="C41" t="s">
         <v>55</v>
@@ -1774,10 +1780,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B42">
-        <v>9357949</v>
+        <v>9283239</v>
       </c>
       <c r="C42" t="s">
         <v>55</v>
@@ -1788,10 +1794,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>263</v>
+        <v>28</v>
       </c>
       <c r="B43">
-        <v>9694581</v>
+        <v>9357949</v>
       </c>
       <c r="C43" t="s">
         <v>55</v>
@@ -1802,13 +1808,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>263</v>
       </c>
       <c r="B44">
-        <v>9355288</v>
+        <v>9694581</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
         <v>62</v>
@@ -1816,10 +1822,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45">
-        <v>9355331</v>
+        <v>9355288</v>
       </c>
       <c r="C45" t="s">
         <v>56</v>
@@ -1830,10 +1836,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B46">
-        <v>9355343</v>
+        <v>9355331</v>
       </c>
       <c r="C46" t="s">
         <v>56</v>
@@ -1844,10 +1850,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B47">
-        <v>9355355</v>
+        <v>9355343</v>
       </c>
       <c r="C47" t="s">
         <v>56</v>
@@ -1858,10 +1864,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>262</v>
+        <v>32</v>
       </c>
       <c r="B48">
-        <v>9355367</v>
+        <v>9355355</v>
       </c>
       <c r="C48" t="s">
         <v>56</v>
@@ -1872,10 +1878,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>262</v>
       </c>
       <c r="B49">
-        <v>9392925</v>
+        <v>9355367</v>
       </c>
       <c r="C49" t="s">
         <v>56</v>
@@ -1886,10 +1892,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>254</v>
+        <v>33</v>
       </c>
       <c r="B50">
-        <v>9394870</v>
+        <v>9392925</v>
       </c>
       <c r="C50" t="s">
         <v>56</v>
@@ -1900,13 +1906,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>34</v>
+        <v>254</v>
       </c>
       <c r="B51">
-        <v>9394882</v>
+        <v>9394870</v>
       </c>
       <c r="C51" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D51" t="s">
         <v>62</v>
@@ -1914,10 +1920,10 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B52">
-        <v>9394894</v>
+        <v>9394882</v>
       </c>
       <c r="C52" t="s">
         <v>57</v>
@@ -1928,10 +1934,10 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>255</v>
+        <v>35</v>
       </c>
       <c r="B53">
-        <v>9402029</v>
+        <v>9394894</v>
       </c>
       <c r="C53" t="s">
         <v>57</v>
@@ -1942,10 +1948,10 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B54">
-        <v>9409352</v>
+        <v>9402029</v>
       </c>
       <c r="C54" t="s">
         <v>57</v>
@@ -1956,13 +1962,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B55">
-        <v>9784257</v>
+        <v>9409352</v>
       </c>
       <c r="C55" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="D55" t="s">
         <v>62</v>
@@ -1970,10 +1976,10 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>36</v>
+        <v>257</v>
       </c>
       <c r="B56">
-        <v>9784269</v>
+        <v>9784257</v>
       </c>
       <c r="C56" t="s">
         <v>3</v>
@@ -1984,10 +1990,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>258</v>
+        <v>36</v>
       </c>
       <c r="B57">
-        <v>9784271</v>
+        <v>9784269</v>
       </c>
       <c r="C57" t="s">
         <v>3</v>
@@ -1998,10 +2004,10 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>37</v>
+        <v>258</v>
       </c>
       <c r="B58">
-        <v>9784283</v>
+        <v>9784271</v>
       </c>
       <c r="C58" t="s">
         <v>3</v>
@@ -2012,10 +2018,10 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B59">
-        <v>9784295</v>
+        <v>9784283</v>
       </c>
       <c r="C59" t="s">
         <v>3</v>
@@ -2026,10 +2032,10 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B60">
-        <v>9784300</v>
+        <v>9784295</v>
       </c>
       <c r="C60" t="s">
         <v>3</v>
@@ -2040,10 +2046,10 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B61">
-        <v>9784312</v>
+        <v>9784300</v>
       </c>
       <c r="C61" t="s">
         <v>3</v>
@@ -2054,10 +2060,10 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B62">
-        <v>9784324</v>
+        <v>9784312</v>
       </c>
       <c r="C62" t="s">
         <v>3</v>
@@ -2068,10 +2074,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>259</v>
+        <v>41</v>
       </c>
       <c r="B63">
-        <v>9784336</v>
+        <v>9784324</v>
       </c>
       <c r="C63" t="s">
         <v>3</v>
@@ -2082,10 +2088,10 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B64">
-        <v>9848948</v>
+        <v>9784336</v>
       </c>
       <c r="C64" t="s">
         <v>3</v>
@@ -2096,10 +2102,10 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>42</v>
+        <v>260</v>
       </c>
       <c r="B65">
-        <v>9848950</v>
+        <v>9848948</v>
       </c>
       <c r="C65" t="s">
         <v>3</v>
@@ -2110,13 +2116,13 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>211</v>
+        <v>42</v>
       </c>
       <c r="B66">
-        <v>9357951</v>
+        <v>9848950</v>
       </c>
       <c r="C66" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="D66" t="s">
         <v>62</v>
@@ -2124,10 +2130,10 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>43</v>
+        <v>211</v>
       </c>
       <c r="B67">
-        <v>9348091</v>
+        <v>9357951</v>
       </c>
       <c r="C67" t="s">
         <v>58</v>
@@ -2138,10 +2144,10 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B68">
-        <v>9357975</v>
+        <v>9348091</v>
       </c>
       <c r="C68" t="s">
         <v>58</v>
@@ -2152,13 +2158,13 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B69">
-        <v>9357963</v>
+        <v>9357975</v>
       </c>
       <c r="C69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D69" t="s">
         <v>62</v>
@@ -2166,10 +2172,10 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B70">
-        <v>9348089</v>
+        <v>9357963</v>
       </c>
       <c r="C70" t="s">
         <v>59</v>
@@ -2180,10 +2186,10 @@
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B71">
-        <v>9348106</v>
+        <v>9348089</v>
       </c>
       <c r="C71" t="s">
         <v>59</v>
@@ -2194,13 +2200,13 @@
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B72">
-        <v>9717228</v>
+        <v>9348106</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D72" t="s">
         <v>62</v>
@@ -2208,10 +2214,10 @@
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B73">
-        <v>9717204</v>
+        <v>9717228</v>
       </c>
       <c r="C73" t="s">
         <v>60</v>
@@ -2222,10 +2228,10 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B74">
-        <v>9717216</v>
+        <v>9717204</v>
       </c>
       <c r="C74" t="s">
         <v>60</v>
@@ -2236,10 +2242,10 @@
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>239</v>
+        <v>50</v>
       </c>
       <c r="B75">
-        <v>9622203</v>
+        <v>9717216</v>
       </c>
       <c r="C75" t="s">
         <v>60</v>
@@ -2250,10 +2256,10 @@
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B76">
-        <v>9622215</v>
+        <v>9622203</v>
       </c>
       <c r="C76" t="s">
         <v>60</v>
@@ -2264,10 +2270,10 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B77">
-        <v>9622227</v>
+        <v>9622215</v>
       </c>
       <c r="C77" t="s">
         <v>60</v>
@@ -2278,10 +2284,10 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B78">
-        <v>9622239</v>
+        <v>9622227</v>
       </c>
       <c r="C78" t="s">
         <v>60</v>
@@ -2292,10 +2298,10 @@
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B79">
-        <v>9622241</v>
+        <v>9622239</v>
       </c>
       <c r="C79" t="s">
         <v>60</v>
@@ -2306,10 +2312,10 @@
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B80">
-        <v>9622253</v>
+        <v>9622241</v>
       </c>
       <c r="C80" t="s">
         <v>60</v>
@@ -2320,13 +2326,13 @@
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>212</v>
+        <v>244</v>
       </c>
       <c r="B81">
-        <v>9778791</v>
+        <v>9622253</v>
       </c>
       <c r="C81" t="s">
-        <v>223</v>
+        <v>60</v>
       </c>
       <c r="D81" t="s">
         <v>62</v>
@@ -2334,10 +2340,10 @@
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B82">
-        <v>9778806</v>
+        <v>9778791</v>
       </c>
       <c r="C82" t="s">
         <v>223</v>
@@ -2348,10 +2354,10 @@
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B83">
-        <v>9778818</v>
+        <v>9778806</v>
       </c>
       <c r="C83" t="s">
         <v>223</v>
@@ -2362,10 +2368,10 @@
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B84">
-        <v>9778820</v>
+        <v>9778818</v>
       </c>
       <c r="C84" t="s">
         <v>223</v>
@@ -2376,10 +2382,10 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B85">
-        <v>9778832</v>
+        <v>9778820</v>
       </c>
       <c r="C85" t="s">
         <v>223</v>
@@ -2390,10 +2396,10 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B86">
-        <v>9778844</v>
+        <v>9778832</v>
       </c>
       <c r="C86" t="s">
         <v>223</v>
@@ -2404,10 +2410,10 @@
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B87">
-        <v>9780445</v>
+        <v>9778844</v>
       </c>
       <c r="C87" t="s">
         <v>223</v>
@@ -2418,10 +2424,10 @@
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B88">
-        <v>9780457</v>
+        <v>9780445</v>
       </c>
       <c r="C88" t="s">
         <v>223</v>
@@ -2432,10 +2438,10 @@
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B89">
-        <v>9780469</v>
+        <v>9780457</v>
       </c>
       <c r="C89" t="s">
         <v>223</v>
@@ -2446,10 +2452,10 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B90">
-        <v>9780471</v>
+        <v>9780469</v>
       </c>
       <c r="C90" t="s">
         <v>223</v>
@@ -2460,10 +2466,10 @@
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B91">
-        <v>9780483</v>
+        <v>9780471</v>
       </c>
       <c r="C91" t="s">
         <v>223</v>
@@ -2474,13 +2480,13 @@
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B92">
-        <v>9775737</v>
+        <v>9780483</v>
       </c>
       <c r="C92" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="D92" t="s">
         <v>62</v>
@@ -2488,10 +2494,10 @@
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B93">
-        <v>9775749</v>
+        <v>9775737</v>
       </c>
       <c r="C93" t="s">
         <v>231</v>
@@ -2502,10 +2508,10 @@
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B94">
-        <v>9775751</v>
+        <v>9775749</v>
       </c>
       <c r="C94" t="s">
         <v>231</v>
@@ -2516,10 +2522,10 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B95">
-        <v>9775763</v>
+        <v>9775751</v>
       </c>
       <c r="C95" t="s">
         <v>231</v>
@@ -2530,10 +2536,10 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B96">
-        <v>9775775</v>
+        <v>9775763</v>
       </c>
       <c r="C96" t="s">
         <v>231</v>
@@ -2544,10 +2550,10 @@
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B97">
-        <v>9778533</v>
+        <v>9775775</v>
       </c>
       <c r="C97" t="s">
         <v>231</v>
@@ -2558,10 +2564,10 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B98">
-        <v>9778545</v>
+        <v>9778533</v>
       </c>
       <c r="C98" t="s">
         <v>231</v>
@@ -2572,24 +2578,24 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>63</v>
+        <v>230</v>
       </c>
       <c r="B99">
-        <v>9525285</v>
+        <v>9778545</v>
       </c>
       <c r="C99" t="s">
-        <v>141</v>
+        <v>231</v>
       </c>
       <c r="D99" t="s">
-        <v>148</v>
+        <v>62</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B100">
-        <v>9525297</v>
+        <v>9525285</v>
       </c>
       <c r="C100" t="s">
         <v>141</v>
@@ -2600,10 +2606,10 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B101">
-        <v>9525302</v>
+        <v>9525297</v>
       </c>
       <c r="C101" t="s">
         <v>141</v>
@@ -2614,10 +2620,10 @@
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B102">
-        <v>9525314</v>
+        <v>9525302</v>
       </c>
       <c r="C102" t="s">
         <v>141</v>
@@ -2628,10 +2634,10 @@
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B103">
-        <v>9525326</v>
+        <v>9525314</v>
       </c>
       <c r="C103" t="s">
         <v>141</v>
@@ -2642,10 +2648,10 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B104">
-        <v>9525338</v>
+        <v>9525326</v>
       </c>
       <c r="C104" t="s">
         <v>141</v>
@@ -2656,10 +2662,10 @@
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B105">
-        <v>9525340</v>
+        <v>9525338</v>
       </c>
       <c r="C105" t="s">
         <v>141</v>
@@ -2670,10 +2676,10 @@
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B106">
-        <v>9525352</v>
+        <v>9525340</v>
       </c>
       <c r="C106" t="s">
         <v>141</v>
@@ -2684,10 +2690,10 @@
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B107">
-        <v>9525364</v>
+        <v>9525352</v>
       </c>
       <c r="C107" t="s">
         <v>141</v>
@@ -2698,10 +2704,10 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B108">
-        <v>9525376</v>
+        <v>9525364</v>
       </c>
       <c r="C108" t="s">
         <v>141</v>
@@ -2712,10 +2718,10 @@
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B109">
-        <v>9525388</v>
+        <v>9525376</v>
       </c>
       <c r="C109" t="s">
         <v>141</v>
@@ -2726,10 +2732,10 @@
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B110">
-        <v>9525390</v>
+        <v>9525388</v>
       </c>
       <c r="C110" t="s">
         <v>141</v>
@@ -2740,10 +2746,10 @@
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B111">
-        <v>9525405</v>
+        <v>9525390</v>
       </c>
       <c r="C111" t="s">
         <v>141</v>
@@ -2754,10 +2760,10 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B112">
-        <v>9525455</v>
+        <v>9525405</v>
       </c>
       <c r="C112" t="s">
         <v>141</v>
@@ -2768,10 +2774,10 @@
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B113">
-        <v>9525467</v>
+        <v>9525455</v>
       </c>
       <c r="C113" t="s">
         <v>141</v>
@@ -2782,10 +2788,10 @@
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B114">
-        <v>9525479</v>
+        <v>9525467</v>
       </c>
       <c r="C114" t="s">
         <v>141</v>
@@ -2796,10 +2802,10 @@
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B115">
-        <v>9525481</v>
+        <v>9525479</v>
       </c>
       <c r="C115" t="s">
         <v>141</v>
@@ -2810,10 +2816,10 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B116">
-        <v>9525493</v>
+        <v>9525481</v>
       </c>
       <c r="C116" t="s">
         <v>141</v>
@@ -2824,10 +2830,10 @@
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B117">
-        <v>9561485</v>
+        <v>9525493</v>
       </c>
       <c r="C117" t="s">
         <v>141</v>
@@ -2838,10 +2844,10 @@
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B118">
-        <v>9561497</v>
+        <v>9561485</v>
       </c>
       <c r="C118" t="s">
         <v>141</v>
@@ -2852,10 +2858,10 @@
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B119">
-        <v>9526459</v>
+        <v>9561497</v>
       </c>
       <c r="C119" t="s">
         <v>141</v>
@@ -2866,10 +2872,10 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B120">
-        <v>9529255</v>
+        <v>9526459</v>
       </c>
       <c r="C120" t="s">
         <v>141</v>
@@ -2880,13 +2886,13 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B121">
-        <v>9321483</v>
+        <v>9529255</v>
       </c>
       <c r="C121" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D121" t="s">
         <v>148</v>
@@ -2894,10 +2900,10 @@
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B122">
-        <v>9321495</v>
+        <v>9321483</v>
       </c>
       <c r="C122" t="s">
         <v>142</v>
@@ -2908,10 +2914,10 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B123">
-        <v>9321500</v>
+        <v>9321495</v>
       </c>
       <c r="C123" t="s">
         <v>142</v>
@@ -2922,10 +2928,10 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B124">
-        <v>9321512</v>
+        <v>9321500</v>
       </c>
       <c r="C124" t="s">
         <v>142</v>
@@ -2936,10 +2942,10 @@
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B125">
-        <v>9321524</v>
+        <v>9321512</v>
       </c>
       <c r="C125" t="s">
         <v>142</v>
@@ -2950,10 +2956,10 @@
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B126">
-        <v>9321536</v>
+        <v>9321524</v>
       </c>
       <c r="C126" t="s">
         <v>142</v>
@@ -2964,10 +2970,10 @@
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B127">
-        <v>9321548</v>
+        <v>9321536</v>
       </c>
       <c r="C127" t="s">
         <v>142</v>
@@ -2978,10 +2984,10 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B128">
-        <v>9321550</v>
+        <v>9321548</v>
       </c>
       <c r="C128" t="s">
         <v>142</v>
@@ -2992,13 +2998,13 @@
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B129">
-        <v>9359002</v>
+        <v>9321550</v>
       </c>
       <c r="C129" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D129" t="s">
         <v>148</v>
@@ -3006,10 +3012,10 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B130">
-        <v>9359014</v>
+        <v>9359002</v>
       </c>
       <c r="C130" t="s">
         <v>143</v>
@@ -3020,10 +3026,10 @@
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B131">
-        <v>9359026</v>
+        <v>9359014</v>
       </c>
       <c r="C131" t="s">
         <v>143</v>
@@ -3034,10 +3040,10 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B132">
-        <v>9359038</v>
+        <v>9359026</v>
       </c>
       <c r="C132" t="s">
         <v>143</v>
@@ -3048,10 +3054,10 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B133">
-        <v>9359040</v>
+        <v>9359038</v>
       </c>
       <c r="C133" t="s">
         <v>143</v>
@@ -3062,10 +3068,10 @@
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B134">
-        <v>9359052</v>
+        <v>9359040</v>
       </c>
       <c r="C134" t="s">
         <v>143</v>
@@ -3076,13 +3082,13 @@
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B135">
-        <v>9302877</v>
+        <v>9359052</v>
       </c>
       <c r="C135" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D135" t="s">
         <v>148</v>
@@ -3090,10 +3096,10 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B136">
-        <v>9302889</v>
+        <v>9302877</v>
       </c>
       <c r="C136" t="s">
         <v>144</v>
@@ -3104,10 +3110,10 @@
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B137">
-        <v>9302891</v>
+        <v>9302889</v>
       </c>
       <c r="C137" t="s">
         <v>144</v>
@@ -3118,10 +3124,10 @@
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B138">
-        <v>9320233</v>
+        <v>9302891</v>
       </c>
       <c r="C138" t="s">
         <v>144</v>
@@ -3132,10 +3138,10 @@
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B139">
-        <v>9320245</v>
+        <v>9320233</v>
       </c>
       <c r="C139" t="s">
         <v>144</v>
@@ -3146,10 +3152,10 @@
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B140">
-        <v>9320257</v>
+        <v>9320245</v>
       </c>
       <c r="C140" t="s">
         <v>144</v>
@@ -3160,13 +3166,13 @@
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B141">
-        <v>9526875</v>
+        <v>9320257</v>
       </c>
       <c r="C141" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D141" t="s">
         <v>148</v>
@@ -3174,10 +3180,10 @@
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B142">
-        <v>9526887</v>
+        <v>9526875</v>
       </c>
       <c r="C142" t="s">
         <v>145</v>
@@ -3188,10 +3194,10 @@
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B143">
-        <v>9526899</v>
+        <v>9526887</v>
       </c>
       <c r="C143" t="s">
         <v>145</v>
@@ -3202,10 +3208,10 @@
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B144">
-        <v>9526904</v>
+        <v>9526899</v>
       </c>
       <c r="C144" t="s">
         <v>145</v>
@@ -3216,10 +3222,10 @@
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B145">
-        <v>9526916</v>
+        <v>9526904</v>
       </c>
       <c r="C145" t="s">
         <v>145</v>
@@ -3230,10 +3236,10 @@
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B146">
-        <v>9526928</v>
+        <v>9526916</v>
       </c>
       <c r="C146" t="s">
         <v>145</v>
@@ -3244,10 +3250,10 @@
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B147">
-        <v>9526930</v>
+        <v>9526928</v>
       </c>
       <c r="C147" t="s">
         <v>145</v>
@@ -3258,10 +3264,10 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B148">
-        <v>9526942</v>
+        <v>9526930</v>
       </c>
       <c r="C148" t="s">
         <v>145</v>
@@ -3272,10 +3278,10 @@
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B149">
-        <v>9526954</v>
+        <v>9526942</v>
       </c>
       <c r="C149" t="s">
         <v>145</v>
@@ -3286,10 +3292,10 @@
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B150">
-        <v>9526966</v>
+        <v>9526954</v>
       </c>
       <c r="C150" t="s">
         <v>145</v>
@@ -3300,10 +3306,10 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B151">
-        <v>9526978</v>
+        <v>9526966</v>
       </c>
       <c r="C151" t="s">
         <v>145</v>
@@ -3314,10 +3320,10 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B152">
-        <v>9527025</v>
+        <v>9526978</v>
       </c>
       <c r="C152" t="s">
         <v>145</v>
@@ -3328,10 +3334,10 @@
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B153">
-        <v>9527037</v>
+        <v>9527025</v>
       </c>
       <c r="C153" t="s">
         <v>145</v>
@@ -3342,10 +3348,10 @@
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B154">
-        <v>9527049</v>
+        <v>9527037</v>
       </c>
       <c r="C154" t="s">
         <v>145</v>
@@ -3356,10 +3362,10 @@
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B155">
-        <v>9527051</v>
+        <v>9527049</v>
       </c>
       <c r="C155" t="s">
         <v>145</v>
@@ -3370,10 +3376,10 @@
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B156">
-        <v>9527063</v>
+        <v>9527051</v>
       </c>
       <c r="C156" t="s">
         <v>145</v>
@@ -3384,13 +3390,13 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B157">
-        <v>9632064</v>
+        <v>9527063</v>
       </c>
       <c r="C157" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D157" t="s">
         <v>148</v>
@@ -3398,10 +3404,10 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B158">
-        <v>9632090</v>
+        <v>9632064</v>
       </c>
       <c r="C158" t="s">
         <v>146</v>
@@ -3412,10 +3418,10 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B159">
-        <v>9632105</v>
+        <v>9632090</v>
       </c>
       <c r="C159" t="s">
         <v>146</v>
@@ -3426,10 +3432,10 @@
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B160">
-        <v>9632117</v>
+        <v>9632105</v>
       </c>
       <c r="C160" t="s">
         <v>146</v>
@@ -3440,10 +3446,10 @@
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B161">
-        <v>9632129</v>
+        <v>9632117</v>
       </c>
       <c r="C161" t="s">
         <v>146</v>
@@ -3454,10 +3460,10 @@
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B162">
-        <v>9632131</v>
+        <v>9632129</v>
       </c>
       <c r="C162" t="s">
         <v>146</v>
@@ -3468,10 +3474,10 @@
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B163">
-        <v>9632143</v>
+        <v>9632131</v>
       </c>
       <c r="C163" t="s">
         <v>146</v>
@@ -3482,10 +3488,10 @@
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B164">
-        <v>9632155</v>
+        <v>9632143</v>
       </c>
       <c r="C164" t="s">
         <v>146</v>
@@ -3496,10 +3502,10 @@
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B165">
-        <v>9632167</v>
+        <v>9632155</v>
       </c>
       <c r="C165" t="s">
         <v>146</v>
@@ -3510,10 +3516,10 @@
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B166">
-        <v>9632179</v>
+        <v>9632167</v>
       </c>
       <c r="C166" t="s">
         <v>146</v>
@@ -3524,13 +3530,13 @@
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B167">
-        <v>9619907</v>
+        <v>9632179</v>
       </c>
       <c r="C167" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D167" t="s">
         <v>148</v>
@@ -3538,10 +3544,10 @@
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B168">
-        <v>9619919</v>
+        <v>9619907</v>
       </c>
       <c r="C168" t="s">
         <v>147</v>
@@ -3552,10 +3558,10 @@
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B169">
-        <v>9619921</v>
+        <v>9619919</v>
       </c>
       <c r="C169" t="s">
         <v>147</v>
@@ -3566,10 +3572,10 @@
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B170">
-        <v>9619933</v>
+        <v>9619921</v>
       </c>
       <c r="C170" t="s">
         <v>147</v>
@@ -3580,10 +3586,10 @@
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B171">
-        <v>9619945</v>
+        <v>9619933</v>
       </c>
       <c r="C171" t="s">
         <v>147</v>
@@ -3594,10 +3600,10 @@
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B172">
-        <v>9619957</v>
+        <v>9619945</v>
       </c>
       <c r="C172" t="s">
         <v>147</v>
@@ -3608,10 +3614,10 @@
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B173">
-        <v>9619969</v>
+        <v>9619957</v>
       </c>
       <c r="C173" t="s">
         <v>147</v>
@@ -3622,10 +3628,10 @@
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B174">
-        <v>9619971</v>
+        <v>9619969</v>
       </c>
       <c r="C174" t="s">
         <v>147</v>
@@ -3636,10 +3642,10 @@
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B175">
-        <v>9619983</v>
+        <v>9619971</v>
       </c>
       <c r="C175" t="s">
         <v>147</v>
@@ -3650,10 +3656,10 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B176">
-        <v>9619995</v>
+        <v>9619983</v>
       </c>
       <c r="C176" t="s">
         <v>147</v>
@@ -3664,24 +3670,24 @@
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B177">
-        <v>9348156</v>
+        <v>9619995</v>
       </c>
       <c r="C177" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D177" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B178">
-        <v>9348168</v>
+        <v>9348156</v>
       </c>
       <c r="C178" t="s">
         <v>158</v>
@@ -3692,10 +3698,10 @@
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B179">
-        <v>9348170</v>
+        <v>9348168</v>
       </c>
       <c r="C179" t="s">
         <v>158</v>
@@ -3706,13 +3712,13 @@
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B180">
-        <v>9456991</v>
+        <v>9348170</v>
       </c>
       <c r="C180" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D180" t="s">
         <v>162</v>
@@ -3720,10 +3726,10 @@
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B181">
-        <v>9457000</v>
+        <v>9456991</v>
       </c>
       <c r="C181" t="s">
         <v>159</v>
@@ -3734,13 +3740,13 @@
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B182">
-        <v>9484560</v>
+        <v>9457000</v>
       </c>
       <c r="C182" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D182" t="s">
         <v>162</v>
@@ -3748,10 +3754,10 @@
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B183">
-        <v>9484572</v>
+        <v>9484560</v>
       </c>
       <c r="C183" t="s">
         <v>160</v>
@@ -3762,13 +3768,13 @@
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B184">
-        <v>9694579</v>
+        <v>9484572</v>
       </c>
       <c r="C184" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D184" t="s">
         <v>162</v>
@@ -3776,10 +3782,10 @@
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B185">
-        <v>9694581</v>
+        <v>9694579</v>
       </c>
       <c r="C185" t="s">
         <v>161</v>
@@ -3790,24 +3796,24 @@
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B186">
-        <v>9342499</v>
+        <v>9694581</v>
       </c>
       <c r="C186" t="s">
-        <v>203</v>
+        <v>161</v>
       </c>
       <c r="D186" t="s">
-        <v>210</v>
+        <v>162</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B187">
-        <v>9342504</v>
+        <v>9342499</v>
       </c>
       <c r="C187" t="s">
         <v>203</v>
@@ -3818,10 +3824,10 @@
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B188">
-        <v>9342516</v>
+        <v>9342504</v>
       </c>
       <c r="C188" t="s">
         <v>203</v>
@@ -3832,10 +3838,10 @@
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B189">
-        <v>9342528</v>
+        <v>9342516</v>
       </c>
       <c r="C189" t="s">
         <v>203</v>
@@ -3846,13 +3852,13 @@
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B190">
-        <v>9298686</v>
+        <v>9342528</v>
       </c>
       <c r="C190" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D190" t="s">
         <v>210</v>
@@ -3860,10 +3866,10 @@
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B191">
-        <v>9298698</v>
+        <v>9298686</v>
       </c>
       <c r="C191" t="s">
         <v>204</v>
@@ -3874,10 +3880,10 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B192">
-        <v>9305300</v>
+        <v>9298698</v>
       </c>
       <c r="C192" t="s">
         <v>204</v>
@@ -3888,10 +3894,10 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B193">
-        <v>9305312</v>
+        <v>9305300</v>
       </c>
       <c r="C193" t="s">
         <v>204</v>
@@ -3902,10 +3908,10 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B194">
-        <v>9311701</v>
+        <v>9305312</v>
       </c>
       <c r="C194" t="s">
         <v>204</v>
@@ -3916,10 +3922,10 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B195">
-        <v>9314210</v>
+        <v>9311701</v>
       </c>
       <c r="C195" t="s">
         <v>204</v>
@@ -3930,10 +3936,10 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B196">
-        <v>9318319</v>
+        <v>9314210</v>
       </c>
       <c r="C196" t="s">
         <v>204</v>
@@ -3944,13 +3950,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B197">
-        <v>9332975</v>
+        <v>9318319</v>
       </c>
       <c r="C197" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D197" t="s">
         <v>210</v>
@@ -3958,10 +3964,10 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B198">
-        <v>9332987</v>
+        <v>9332975</v>
       </c>
       <c r="C198" t="s">
         <v>205</v>
@@ -3972,10 +3978,10 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B199">
-        <v>9332999</v>
+        <v>9332987</v>
       </c>
       <c r="C199" t="s">
         <v>205</v>
@@ -3986,10 +3992,10 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B200">
-        <v>9333008</v>
+        <v>9332999</v>
       </c>
       <c r="C200" t="s">
         <v>205</v>
@@ -4000,10 +4006,10 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B201">
-        <v>9333010</v>
+        <v>9333008</v>
       </c>
       <c r="C201" t="s">
         <v>205</v>
@@ -4014,10 +4020,10 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B202">
-        <v>9333022</v>
+        <v>9333010</v>
       </c>
       <c r="C202" t="s">
         <v>205</v>
@@ -4028,10 +4034,10 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B203">
-        <v>9333034</v>
+        <v>9333022</v>
       </c>
       <c r="C203" t="s">
         <v>205</v>
@@ -4042,10 +4048,10 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B204">
-        <v>9342176</v>
+        <v>9333034</v>
       </c>
       <c r="C204" t="s">
         <v>205</v>
@@ -4056,10 +4062,10 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B205">
-        <v>9348649</v>
+        <v>9342176</v>
       </c>
       <c r="C205" t="s">
         <v>205</v>
@@ -4070,10 +4076,10 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B206">
-        <v>9348651</v>
+        <v>9348649</v>
       </c>
       <c r="C206" t="s">
         <v>205</v>
@@ -4084,13 +4090,13 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B207">
-        <v>9294379</v>
+        <v>9348651</v>
       </c>
       <c r="C207" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D207" t="s">
         <v>210</v>
@@ -4098,10 +4104,10 @@
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B208">
-        <v>9294381</v>
+        <v>9294379</v>
       </c>
       <c r="C208" t="s">
         <v>206</v>
@@ -4112,10 +4118,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B209">
-        <v>9294393</v>
+        <v>9294381</v>
       </c>
       <c r="C209" t="s">
         <v>206</v>
@@ -4126,13 +4132,13 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B210">
-        <v>9315197</v>
+        <v>9294393</v>
       </c>
       <c r="C210" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D210" t="s">
         <v>210</v>
@@ -4140,10 +4146,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B211">
-        <v>9315202</v>
+        <v>9315197</v>
       </c>
       <c r="C211" t="s">
         <v>207</v>
@@ -4154,10 +4160,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B212">
-        <v>9315214</v>
+        <v>9315202</v>
       </c>
       <c r="C212" t="s">
         <v>207</v>
@@ -4168,10 +4174,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B213">
-        <v>9315226</v>
+        <v>9315214</v>
       </c>
       <c r="C213" t="s">
         <v>207</v>
@@ -4182,10 +4188,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B214">
-        <v>9315238</v>
+        <v>9315226</v>
       </c>
       <c r="C214" t="s">
         <v>207</v>
@@ -4196,10 +4202,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B215">
-        <v>9315240</v>
+        <v>9315238</v>
       </c>
       <c r="C215" t="s">
         <v>207</v>
@@ -4210,10 +4216,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B216">
-        <v>9315252</v>
+        <v>9315240</v>
       </c>
       <c r="C216" t="s">
         <v>207</v>
@@ -4224,13 +4230,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B217">
-        <v>9352004</v>
+        <v>9315252</v>
       </c>
       <c r="C217" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D217" t="s">
         <v>210</v>
@@ -4238,10 +4244,10 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B218">
-        <v>9352016</v>
+        <v>9352004</v>
       </c>
       <c r="C218" t="s">
         <v>208</v>
@@ -4252,10 +4258,10 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B219">
-        <v>9352028</v>
+        <v>9352016</v>
       </c>
       <c r="C219" t="s">
         <v>208</v>
@@ -4266,10 +4272,10 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B220">
-        <v>9352030</v>
+        <v>9352028</v>
       </c>
       <c r="C220" t="s">
         <v>208</v>
@@ -4280,10 +4286,10 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B221">
-        <v>9352042</v>
+        <v>9352030</v>
       </c>
       <c r="C221" t="s">
         <v>208</v>
@@ -4294,13 +4300,13 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B222">
-        <v>9332511</v>
+        <v>9352042</v>
       </c>
       <c r="C222" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D222" t="s">
         <v>210</v>
@@ -4308,10 +4314,10 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B223">
-        <v>9334662</v>
+        <v>9332511</v>
       </c>
       <c r="C223" t="s">
         <v>209</v>
@@ -4322,10 +4328,10 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B224">
-        <v>9334674</v>
+        <v>9334662</v>
       </c>
       <c r="C224" t="s">
         <v>209</v>
@@ -4336,15 +4342,29 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B225">
-        <v>9334686</v>
+        <v>9334674</v>
       </c>
       <c r="C225" t="s">
         <v>209</v>
       </c>
       <c r="D225" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A226" t="s">
+        <v>202</v>
+      </c>
+      <c r="B226">
+        <v>9334686</v>
+      </c>
+      <c r="C226" t="s">
+        <v>209</v>
+      </c>
+      <c r="D226" t="s">
         <v>210</v>
       </c>
     </row>

</xml_diff>

<commit_message>
"Changed Monte Alto to Monte Sarmiento"
</commit_message>
<xml_diff>
--- a/trackedvessels.xlsx
+++ b/trackedvessels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/Vesseltimeline/VesselTimeline_dataGet-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A24BFF1-5C75-41B9-827F-ED0F7983FF93}"/>
+  <xr:revisionPtr revIDLastSave="151" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A4D3646B-A86D-4917-A098-5DE6F30BC6BB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="51420" windowHeight="13900" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
+    <workbookView xWindow="25510" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="264">
   <si>
     <t>Santa Rosa</t>
   </si>
@@ -828,12 +828,6 @@
   </si>
   <si>
     <t>Monte Sarmiento</t>
-  </si>
-  <si>
-    <t>Monte Alto</t>
-  </si>
-  <si>
-    <t>Monte</t>
   </si>
 </sst>
 </file>
@@ -1193,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A49309-98C8-6143-85DD-C6C0E46E1D27}">
   <dimension ref="A1:D226"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1430,13 +1424,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B17">
         <v>9283227</v>
       </c>
       <c r="C17" t="s">
-        <v>265</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
"Print statement for monte alto"
</commit_message>
<xml_diff>
--- a/trackedvessels.xlsx
+++ b/trackedvessels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/Vesseltimeline/VesselTimeline_dataGet-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3E69A04-8ED4-43B1-8AF3-90956443DED7}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FEEC025-4759-471A-872C-1065A073328E}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="0" windowWidth="38400" windowHeight="9920" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
+    <workbookView xWindow="25510" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -827,10 +827,10 @@
     <t>Safmarine Benguela</t>
   </si>
   <si>
-    <t>Monte Sarmiento</t>
-  </si>
-  <si>
     <t>Maersk Monte Alto</t>
+  </si>
+  <si>
+    <t>Monte Ganges</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1191,7 @@
   <dimension ref="A1:D226"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A44" sqref="A44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B37">
         <v>9283227</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B44">
         <v>9694581</v>

</xml_diff>

<commit_message>
"Monte alto (Sarmiento) added, dataget.py back"
</commit_message>
<xml_diff>
--- a/trackedvessels.xlsx
+++ b/trackedvessels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/Vesseltimeline/VesselTimeline_dataGet-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FEEC025-4759-471A-872C-1065A073328E}"/>
+  <xr:revisionPtr revIDLastSave="157" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD8374C1-2814-44FB-81D5-BAF7A777A473}"/>
   <bookViews>
-    <workbookView xWindow="25510" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
+    <workbookView xWindow="1530" yWindow="0" windowWidth="38400" windowHeight="9920" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -827,10 +827,10 @@
     <t>Safmarine Benguela</t>
   </si>
   <si>
-    <t>Maersk Monte Alto</t>
-  </si>
-  <si>
     <t>Monte Ganges</t>
+  </si>
+  <si>
+    <t>Monte Alto</t>
   </si>
 </sst>
 </file>
@@ -1191,7 +1191,7 @@
   <dimension ref="A1:D226"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B37">
         <v>9283227</v>
@@ -1805,7 +1805,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B44">
         <v>9694581</v>

</xml_diff>

<commit_message>
"Added vessels not in projects"
</commit_message>
<xml_diff>
--- a/trackedvessels.xlsx
+++ b/trackedvessels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/Vesseltimeline/VesselTimeline_dataGet-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD8374C1-2814-44FB-81D5-BAF7A777A473}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCC9EFE0-369D-448D-B63B-CD1CF27E9909}"/>
   <bookViews>
-    <workbookView xWindow="1530" yWindow="0" windowWidth="38400" windowHeight="9920" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
+    <workbookView xWindow="-100" yWindow="0" windowWidth="25800" windowHeight="13780" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="267">
   <si>
     <t>Santa Rosa</t>
   </si>
@@ -831,6 +831,12 @@
   </si>
   <si>
     <t>Monte Alto</t>
+  </si>
+  <si>
+    <t>Maersk</t>
+  </si>
+  <si>
+    <t>Maersk vessels not in projects</t>
   </si>
 </sst>
 </file>
@@ -1188,10 +1194,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A49309-98C8-6143-85DD-C6C0E46E1D27}">
-  <dimension ref="A1:D226"/>
+  <dimension ref="A1:D400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="E225" sqref="E225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4365,6 +4371,1920 @@
         <v>210</v>
       </c>
     </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B227">
+        <v>9260445</v>
+      </c>
+      <c r="C227" t="s">
+        <v>266</v>
+      </c>
+      <c r="D227" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B228">
+        <v>9214903</v>
+      </c>
+      <c r="C228" t="s">
+        <v>266</v>
+      </c>
+      <c r="D228" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B229">
+        <v>9219795</v>
+      </c>
+      <c r="C229" t="s">
+        <v>266</v>
+      </c>
+      <c r="D229" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B230">
+        <v>9245744</v>
+      </c>
+      <c r="C230" t="s">
+        <v>266</v>
+      </c>
+      <c r="D230" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B231">
+        <v>9219800</v>
+      </c>
+      <c r="C231" t="s">
+        <v>266</v>
+      </c>
+      <c r="D231" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B232">
+        <v>9245770</v>
+      </c>
+      <c r="C232" t="s">
+        <v>266</v>
+      </c>
+      <c r="D232" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B233">
+        <v>9198575</v>
+      </c>
+      <c r="C233" t="s">
+        <v>266</v>
+      </c>
+      <c r="D233" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B234">
+        <v>9245768</v>
+      </c>
+      <c r="C234" t="s">
+        <v>266</v>
+      </c>
+      <c r="D234" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B235">
+        <v>9245756</v>
+      </c>
+      <c r="C235" t="s">
+        <v>266</v>
+      </c>
+      <c r="D235" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B236">
+        <v>9198587</v>
+      </c>
+      <c r="C236" t="s">
+        <v>266</v>
+      </c>
+      <c r="D236" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B237">
+        <v>9193276</v>
+      </c>
+      <c r="C237" t="s">
+        <v>266</v>
+      </c>
+      <c r="D237" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B238">
+        <v>9215177</v>
+      </c>
+      <c r="C238" t="s">
+        <v>266</v>
+      </c>
+      <c r="D238" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B239">
+        <v>9215189</v>
+      </c>
+      <c r="C239" t="s">
+        <v>266</v>
+      </c>
+      <c r="D239" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B240">
+        <v>9215191</v>
+      </c>
+      <c r="C240" t="s">
+        <v>266</v>
+      </c>
+      <c r="D240" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B241">
+        <v>9190743</v>
+      </c>
+      <c r="C241" t="s">
+        <v>266</v>
+      </c>
+      <c r="D241" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B242">
+        <v>9190755</v>
+      </c>
+      <c r="C242" t="s">
+        <v>266</v>
+      </c>
+      <c r="D242" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B243">
+        <v>9190767</v>
+      </c>
+      <c r="C243" t="s">
+        <v>266</v>
+      </c>
+      <c r="D243" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B244">
+        <v>9190779</v>
+      </c>
+      <c r="C244" t="s">
+        <v>266</v>
+      </c>
+      <c r="D244" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B245">
+        <v>9190731</v>
+      </c>
+      <c r="C245" t="s">
+        <v>266</v>
+      </c>
+      <c r="D245" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="246" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B246">
+        <v>9190781</v>
+      </c>
+      <c r="C246" t="s">
+        <v>266</v>
+      </c>
+      <c r="D246" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="247" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B247">
+        <v>9928188</v>
+      </c>
+      <c r="C247" t="s">
+        <v>266</v>
+      </c>
+      <c r="D247" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="248" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B248">
+        <v>9398395</v>
+      </c>
+      <c r="C248" t="s">
+        <v>266</v>
+      </c>
+      <c r="D248" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B249">
+        <v>9175781</v>
+      </c>
+      <c r="C249" t="s">
+        <v>266</v>
+      </c>
+      <c r="D249" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="250" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B250">
+        <v>9624275</v>
+      </c>
+      <c r="C250" t="s">
+        <v>266</v>
+      </c>
+      <c r="D250" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B251">
+        <v>9398424</v>
+      </c>
+      <c r="C251" t="s">
+        <v>266</v>
+      </c>
+      <c r="D251" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B252">
+        <v>9164275</v>
+      </c>
+      <c r="C252" t="s">
+        <v>266</v>
+      </c>
+      <c r="D252" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B253">
+        <v>9697026</v>
+      </c>
+      <c r="C253" t="s">
+        <v>266</v>
+      </c>
+      <c r="D253" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B254">
+        <v>9313917</v>
+      </c>
+      <c r="C254" t="s">
+        <v>266</v>
+      </c>
+      <c r="D254" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B255">
+        <v>9313929</v>
+      </c>
+      <c r="C255" t="s">
+        <v>266</v>
+      </c>
+      <c r="D255" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B256">
+        <v>9697014</v>
+      </c>
+      <c r="C256" t="s">
+        <v>266</v>
+      </c>
+      <c r="D256" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="257" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B257">
+        <v>9840702</v>
+      </c>
+      <c r="C257" t="s">
+        <v>266</v>
+      </c>
+      <c r="D257" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="258" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B258">
+        <v>9928190</v>
+      </c>
+      <c r="C258" t="s">
+        <v>266</v>
+      </c>
+      <c r="D258" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="259" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B259">
+        <v>9313905</v>
+      </c>
+      <c r="C259" t="s">
+        <v>266</v>
+      </c>
+      <c r="D259" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="260" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B260">
+        <v>9313931</v>
+      </c>
+      <c r="C260" t="s">
+        <v>266</v>
+      </c>
+      <c r="D260" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="261" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B261">
+        <v>9313955</v>
+      </c>
+      <c r="C261" t="s">
+        <v>266</v>
+      </c>
+      <c r="D261" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="262" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B262">
+        <v>9924182</v>
+      </c>
+      <c r="C262" t="s">
+        <v>266</v>
+      </c>
+      <c r="D262" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="263" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B263">
+        <v>9924194</v>
+      </c>
+      <c r="C263" t="s">
+        <v>266</v>
+      </c>
+      <c r="D263" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="264" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B264">
+        <v>9924209</v>
+      </c>
+      <c r="C264" t="s">
+        <v>266</v>
+      </c>
+      <c r="D264" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B265">
+        <v>9924211</v>
+      </c>
+      <c r="C265" t="s">
+        <v>266</v>
+      </c>
+      <c r="D265" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="266" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B266">
+        <v>9924223</v>
+      </c>
+      <c r="C266" t="s">
+        <v>266</v>
+      </c>
+      <c r="D266" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="267" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B267">
+        <v>9924235</v>
+      </c>
+      <c r="C267" t="s">
+        <v>266</v>
+      </c>
+      <c r="D267" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="268" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B268">
+        <v>9761023</v>
+      </c>
+      <c r="C268" t="s">
+        <v>266</v>
+      </c>
+      <c r="D268" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="269" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B269">
+        <v>9356074</v>
+      </c>
+      <c r="C269" t="s">
+        <v>266</v>
+      </c>
+      <c r="D269" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="270" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B270">
+        <v>9302449</v>
+      </c>
+      <c r="C270" t="s">
+        <v>266</v>
+      </c>
+      <c r="D270" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="271" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B271">
+        <v>9858711</v>
+      </c>
+      <c r="C271" t="s">
+        <v>266</v>
+      </c>
+      <c r="D271" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="272" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B272">
+        <v>9871165</v>
+      </c>
+      <c r="C272" t="s">
+        <v>266</v>
+      </c>
+      <c r="D272" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="273" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B273">
+        <v>9299032</v>
+      </c>
+      <c r="C273" t="s">
+        <v>266</v>
+      </c>
+      <c r="D273" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="274" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B274">
+        <v>9299044</v>
+      </c>
+      <c r="C274" t="s">
+        <v>266</v>
+      </c>
+      <c r="D274" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="275" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B275">
+        <v>9502867</v>
+      </c>
+      <c r="C275" t="s">
+        <v>266</v>
+      </c>
+      <c r="D275" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="276" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B276">
+        <v>9458030</v>
+      </c>
+      <c r="C276" t="s">
+        <v>266</v>
+      </c>
+      <c r="D276" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="277" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B277">
+        <v>9502910</v>
+      </c>
+      <c r="C277" t="s">
+        <v>266</v>
+      </c>
+      <c r="D277" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="278" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B278">
+        <v>9502958</v>
+      </c>
+      <c r="C278" t="s">
+        <v>266</v>
+      </c>
+      <c r="D278" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="279" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B279">
+        <v>9502946</v>
+      </c>
+      <c r="C279" t="s">
+        <v>266</v>
+      </c>
+      <c r="D279" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="280" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B280">
+        <v>9502972</v>
+      </c>
+      <c r="C280" t="s">
+        <v>266</v>
+      </c>
+      <c r="D280" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="281" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B281">
+        <v>9694567</v>
+      </c>
+      <c r="C281" t="s">
+        <v>266</v>
+      </c>
+      <c r="D281" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="282" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B282">
+        <v>9501239</v>
+      </c>
+      <c r="C282" t="s">
+        <v>266</v>
+      </c>
+      <c r="D282" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="283" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B283">
+        <v>9928205</v>
+      </c>
+      <c r="C283" t="s">
+        <v>266</v>
+      </c>
+      <c r="D283" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="284" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B284">
+        <v>9235567</v>
+      </c>
+      <c r="C284" t="s">
+        <v>266</v>
+      </c>
+      <c r="D284" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="285" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B285">
+        <v>9235579</v>
+      </c>
+      <c r="C285" t="s">
+        <v>266</v>
+      </c>
+      <c r="D285" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="286" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B286">
+        <v>9235543</v>
+      </c>
+      <c r="C286" t="s">
+        <v>266</v>
+      </c>
+      <c r="D286" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="287" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B287">
+        <v>9739680</v>
+      </c>
+      <c r="C287" t="s">
+        <v>266</v>
+      </c>
+      <c r="D287" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="288" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B288">
+        <v>9739692</v>
+      </c>
+      <c r="C288" t="s">
+        <v>266</v>
+      </c>
+      <c r="D288" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="289" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B289">
+        <v>9235555</v>
+      </c>
+      <c r="C289" t="s">
+        <v>266</v>
+      </c>
+      <c r="D289" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="290" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B290">
+        <v>9713375</v>
+      </c>
+      <c r="C290" t="s">
+        <v>266</v>
+      </c>
+      <c r="D290" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="291" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B291">
+        <v>9727871</v>
+      </c>
+      <c r="C291" t="s">
+        <v>266</v>
+      </c>
+      <c r="D291" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="292" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B292">
+        <v>9858735</v>
+      </c>
+      <c r="C292" t="s">
+        <v>266</v>
+      </c>
+      <c r="D292" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="293" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B293">
+        <v>9193264</v>
+      </c>
+      <c r="C293" t="s">
+        <v>266</v>
+      </c>
+      <c r="D293" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="294" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B294">
+        <v>9329629</v>
+      </c>
+      <c r="C294" t="s">
+        <v>266</v>
+      </c>
+      <c r="D294" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="295" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B295">
+        <v>9624287</v>
+      </c>
+      <c r="C295" t="s">
+        <v>266</v>
+      </c>
+      <c r="D295" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="296" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B296">
+        <v>9343077</v>
+      </c>
+      <c r="C296" t="s">
+        <v>266</v>
+      </c>
+      <c r="D296" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="297" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B297">
+        <v>9343974</v>
+      </c>
+      <c r="C297" t="s">
+        <v>266</v>
+      </c>
+      <c r="D297" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="298" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B298">
+        <v>9865881</v>
+      </c>
+      <c r="C298" t="s">
+        <v>266</v>
+      </c>
+      <c r="D298" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="299" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B299">
+        <v>9294161</v>
+      </c>
+      <c r="C299" t="s">
+        <v>266</v>
+      </c>
+      <c r="D299" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="300" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B300">
+        <v>9360245</v>
+      </c>
+      <c r="C300" t="s">
+        <v>266</v>
+      </c>
+      <c r="D300" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="301" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B301">
+        <v>9162215</v>
+      </c>
+      <c r="C301" t="s">
+        <v>266</v>
+      </c>
+      <c r="D301" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="302" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B302">
+        <v>9624299</v>
+      </c>
+      <c r="C302" t="s">
+        <v>266</v>
+      </c>
+      <c r="D302" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="303" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B303">
+        <v>9193240</v>
+      </c>
+      <c r="C303" t="s">
+        <v>266</v>
+      </c>
+      <c r="D303" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="304" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B304">
+        <v>9290476</v>
+      </c>
+      <c r="C304" t="s">
+        <v>266</v>
+      </c>
+      <c r="D304" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="305" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B305">
+        <v>9858747</v>
+      </c>
+      <c r="C305" t="s">
+        <v>266</v>
+      </c>
+      <c r="D305" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="306" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B306">
+        <v>9840738</v>
+      </c>
+      <c r="C306" t="s">
+        <v>266</v>
+      </c>
+      <c r="D306" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="307" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B307">
+        <v>9459424</v>
+      </c>
+      <c r="C307" t="s">
+        <v>266</v>
+      </c>
+      <c r="D307" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="308" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B308">
+        <v>9893864</v>
+      </c>
+      <c r="C308" t="s">
+        <v>266</v>
+      </c>
+      <c r="D308" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="309" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B309">
+        <v>9386017</v>
+      </c>
+      <c r="C309" t="s">
+        <v>266</v>
+      </c>
+      <c r="D309" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="310" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B310">
+        <v>9356165</v>
+      </c>
+      <c r="C310" t="s">
+        <v>266</v>
+      </c>
+      <c r="D310" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="311" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B311">
+        <v>9385996</v>
+      </c>
+      <c r="C311" t="s">
+        <v>266</v>
+      </c>
+      <c r="D311" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="312" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B312">
+        <v>9356098</v>
+      </c>
+      <c r="C312" t="s">
+        <v>266</v>
+      </c>
+      <c r="D312" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="313" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B313">
+        <v>9894648</v>
+      </c>
+      <c r="C313" t="s">
+        <v>266</v>
+      </c>
+      <c r="D313" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="314" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B314">
+        <v>9893876</v>
+      </c>
+      <c r="C314" t="s">
+        <v>266</v>
+      </c>
+      <c r="D314" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="315" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B315">
+        <v>9894650</v>
+      </c>
+      <c r="C315" t="s">
+        <v>266</v>
+      </c>
+      <c r="D315" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="316" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B316">
+        <v>9215907</v>
+      </c>
+      <c r="C316" t="s">
+        <v>266</v>
+      </c>
+      <c r="D316" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="317" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B317">
+        <v>9402627</v>
+      </c>
+      <c r="C317" t="s">
+        <v>266</v>
+      </c>
+      <c r="D317" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="318" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B318">
+        <v>9402615</v>
+      </c>
+      <c r="C318" t="s">
+        <v>266</v>
+      </c>
+      <c r="D318" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="319" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B319">
+        <v>9231470</v>
+      </c>
+      <c r="C319" t="s">
+        <v>266</v>
+      </c>
+      <c r="D319" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="320" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B320">
+        <v>9215878</v>
+      </c>
+      <c r="C320" t="s">
+        <v>266</v>
+      </c>
+      <c r="D320" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="321" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B321">
+        <v>9215880</v>
+      </c>
+      <c r="C321" t="s">
+        <v>266</v>
+      </c>
+      <c r="D321" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="322" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B322">
+        <v>9356127</v>
+      </c>
+      <c r="C322" t="s">
+        <v>266</v>
+      </c>
+      <c r="D322" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="323" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B323">
+        <v>9385972</v>
+      </c>
+      <c r="C323" t="s">
+        <v>266</v>
+      </c>
+      <c r="D323" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="324" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B324">
+        <v>9402639</v>
+      </c>
+      <c r="C324" t="s">
+        <v>266</v>
+      </c>
+      <c r="D324" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="325" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B325">
+        <v>9893852</v>
+      </c>
+      <c r="C325" t="s">
+        <v>266</v>
+      </c>
+      <c r="D325" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="326" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B326">
+        <v>9894674</v>
+      </c>
+      <c r="C326" t="s">
+        <v>266</v>
+      </c>
+      <c r="D326" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="327" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B327">
+        <v>9894686</v>
+      </c>
+      <c r="C327" t="s">
+        <v>266</v>
+      </c>
+      <c r="D327" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="328" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B328">
+        <v>9356139</v>
+      </c>
+      <c r="C328" t="s">
+        <v>266</v>
+      </c>
+      <c r="D328" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="329" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B329">
+        <v>9215919</v>
+      </c>
+      <c r="C329" t="s">
+        <v>266</v>
+      </c>
+      <c r="D329" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="330" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B330">
+        <v>9222118</v>
+      </c>
+      <c r="C330" t="s">
+        <v>266</v>
+      </c>
+      <c r="D330" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="331" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B331">
+        <v>9306172</v>
+      </c>
+      <c r="C331" t="s">
+        <v>266</v>
+      </c>
+      <c r="D331" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="332" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B332">
+        <v>9840714</v>
+      </c>
+      <c r="C332" t="s">
+        <v>266</v>
+      </c>
+      <c r="D332" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="333" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B333">
+        <v>9740457</v>
+      </c>
+      <c r="C333" t="s">
+        <v>266</v>
+      </c>
+      <c r="D333" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="334" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B334">
+        <v>9840726</v>
+      </c>
+      <c r="C334" t="s">
+        <v>266</v>
+      </c>
+      <c r="D334" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="335" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B335">
+        <v>9726671</v>
+      </c>
+      <c r="C335" t="s">
+        <v>266</v>
+      </c>
+      <c r="D335" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="336" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B336">
+        <v>9344954</v>
+      </c>
+      <c r="C336" t="s">
+        <v>266</v>
+      </c>
+      <c r="D336" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="337" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B337">
+        <v>9833369</v>
+      </c>
+      <c r="C337" t="s">
+        <v>266</v>
+      </c>
+      <c r="D337" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="338" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B338">
+        <v>9411381</v>
+      </c>
+      <c r="C338" t="s">
+        <v>266</v>
+      </c>
+      <c r="D338" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="339" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B339">
+        <v>9433054</v>
+      </c>
+      <c r="C339" t="s">
+        <v>266</v>
+      </c>
+      <c r="D339" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="340" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B340">
+        <v>9411379</v>
+      </c>
+      <c r="C340" t="s">
+        <v>266</v>
+      </c>
+      <c r="D340" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="341" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B341">
+        <v>9344681</v>
+      </c>
+      <c r="C341" t="s">
+        <v>266</v>
+      </c>
+      <c r="D341" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="342" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B342">
+        <v>9436173</v>
+      </c>
+      <c r="C342" t="s">
+        <v>266</v>
+      </c>
+      <c r="D342" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="343" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B343">
+        <v>9436185</v>
+      </c>
+      <c r="C343" t="s">
+        <v>266</v>
+      </c>
+      <c r="D343" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="344" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B344">
+        <v>9401697</v>
+      </c>
+      <c r="C344" t="s">
+        <v>266</v>
+      </c>
+      <c r="D344" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="345" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B345">
+        <v>9408956</v>
+      </c>
+      <c r="C345" t="s">
+        <v>266</v>
+      </c>
+      <c r="D345" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="346" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B346">
+        <v>9235531</v>
+      </c>
+      <c r="C346" t="s">
+        <v>266</v>
+      </c>
+      <c r="D346" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="347" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B347">
+        <v>9411367</v>
+      </c>
+      <c r="C347" t="s">
+        <v>266</v>
+      </c>
+      <c r="D347" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="348" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B348">
+        <v>9840697</v>
+      </c>
+      <c r="C348" t="s">
+        <v>266</v>
+      </c>
+      <c r="D348" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="349" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B349">
+        <v>9550357</v>
+      </c>
+      <c r="C349" t="s">
+        <v>266</v>
+      </c>
+      <c r="D349" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="350" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B350">
+        <v>9459632</v>
+      </c>
+      <c r="C350" t="s">
+        <v>266</v>
+      </c>
+      <c r="D350" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="351" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B351">
+        <v>9391660</v>
+      </c>
+      <c r="C351" t="s">
+        <v>266</v>
+      </c>
+      <c r="D351" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="352" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B352">
+        <v>9362401</v>
+      </c>
+      <c r="C352" t="s">
+        <v>266</v>
+      </c>
+      <c r="D352" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="353" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B353">
+        <v>9858723</v>
+      </c>
+      <c r="C353" t="s">
+        <v>266</v>
+      </c>
+      <c r="D353" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="354" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B354">
+        <v>9289192</v>
+      </c>
+      <c r="C354" t="s">
+        <v>266</v>
+      </c>
+      <c r="D354" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="355" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B355">
+        <v>9398436</v>
+      </c>
+      <c r="C355" t="s">
+        <v>266</v>
+      </c>
+      <c r="D355" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="356" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B356">
+        <v>9786085</v>
+      </c>
+      <c r="C356" t="s">
+        <v>266</v>
+      </c>
+      <c r="D356" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="357" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B357">
+        <v>9885130</v>
+      </c>
+      <c r="C357" t="s">
+        <v>266</v>
+      </c>
+      <c r="D357" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="358" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B358">
+        <v>9192442</v>
+      </c>
+      <c r="C358" t="s">
+        <v>266</v>
+      </c>
+      <c r="D358" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="359" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B359">
+        <v>9220885</v>
+      </c>
+      <c r="C359" t="s">
+        <v>266</v>
+      </c>
+      <c r="D359" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="360" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B360">
+        <v>9192454</v>
+      </c>
+      <c r="C360" t="s">
+        <v>266</v>
+      </c>
+      <c r="D360" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="361" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B361">
+        <v>9192466</v>
+      </c>
+      <c r="C361" t="s">
+        <v>266</v>
+      </c>
+      <c r="D361" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="362" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B362">
+        <v>9885166</v>
+      </c>
+      <c r="C362" t="s">
+        <v>266</v>
+      </c>
+      <c r="D362" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="363" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B363">
+        <v>9192478</v>
+      </c>
+      <c r="C363" t="s">
+        <v>266</v>
+      </c>
+      <c r="D363" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="364" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B364">
+        <v>9885154</v>
+      </c>
+      <c r="C364" t="s">
+        <v>266</v>
+      </c>
+      <c r="D364" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="365" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B365">
+        <v>9885142</v>
+      </c>
+      <c r="C365" t="s">
+        <v>266</v>
+      </c>
+      <c r="D365" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="366" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B366">
+        <v>9885178</v>
+      </c>
+      <c r="C366" t="s">
+        <v>266</v>
+      </c>
+      <c r="D366" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="367" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B367">
+        <v>9220897</v>
+      </c>
+      <c r="C367" t="s">
+        <v>266</v>
+      </c>
+      <c r="D367" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="368" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B368">
+        <v>9251614</v>
+      </c>
+      <c r="C368" t="s">
+        <v>266</v>
+      </c>
+      <c r="D368" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="369" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B369">
+        <v>9251638</v>
+      </c>
+      <c r="C369" t="s">
+        <v>266</v>
+      </c>
+      <c r="D369" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="370" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B370">
+        <v>9251626</v>
+      </c>
+      <c r="C370" t="s">
+        <v>266</v>
+      </c>
+      <c r="D370" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="371" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B371">
+        <v>9120865</v>
+      </c>
+      <c r="C371" t="s">
+        <v>266</v>
+      </c>
+      <c r="D371" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="372" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B372">
+        <v>9166792</v>
+      </c>
+      <c r="C372" t="s">
+        <v>266</v>
+      </c>
+      <c r="D372" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="373" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B373">
+        <v>9499022</v>
+      </c>
+      <c r="C373" t="s">
+        <v>266</v>
+      </c>
+      <c r="D373" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="374" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B374">
+        <v>9332690</v>
+      </c>
+      <c r="C374" t="s">
+        <v>266</v>
+      </c>
+      <c r="D374" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="375" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B375">
+        <v>9823730</v>
+      </c>
+      <c r="C375" t="s">
+        <v>266</v>
+      </c>
+      <c r="D375" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="376" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B376">
+        <v>9823742</v>
+      </c>
+      <c r="C376" t="s">
+        <v>266</v>
+      </c>
+      <c r="D376" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="377" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B377">
+        <v>9332705</v>
+      </c>
+      <c r="C377" t="s">
+        <v>266</v>
+      </c>
+      <c r="D377" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="378" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B378">
+        <v>9634696</v>
+      </c>
+      <c r="C378" t="s">
+        <v>266</v>
+      </c>
+      <c r="D378" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="379" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B379">
+        <v>9823766</v>
+      </c>
+      <c r="C379" t="s">
+        <v>266</v>
+      </c>
+      <c r="D379" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="380" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B380">
+        <v>9823728</v>
+      </c>
+      <c r="C380" t="s">
+        <v>266</v>
+      </c>
+      <c r="D380" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="381" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B381">
+        <v>9823754</v>
+      </c>
+      <c r="C381" t="s">
+        <v>266</v>
+      </c>
+      <c r="D381" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="382" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B382">
+        <v>9936379</v>
+      </c>
+      <c r="C382" t="s">
+        <v>266</v>
+      </c>
+      <c r="D382" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="383" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B383">
+        <v>9936410</v>
+      </c>
+      <c r="C383" t="s">
+        <v>266</v>
+      </c>
+      <c r="D383" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="384" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B384">
+        <v>9936408</v>
+      </c>
+      <c r="C384" t="s">
+        <v>266</v>
+      </c>
+      <c r="D384" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="385" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B385">
+        <v>9964481</v>
+      </c>
+      <c r="C385" t="s">
+        <v>266</v>
+      </c>
+      <c r="D385" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="386" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B386">
+        <v>9969041</v>
+      </c>
+      <c r="C386" t="s">
+        <v>266</v>
+      </c>
+      <c r="D386" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="387" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B387">
+        <v>9928217</v>
+      </c>
+      <c r="C387" t="s">
+        <v>266</v>
+      </c>
+      <c r="D387" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="388" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B388">
+        <v>9966128</v>
+      </c>
+      <c r="C388" t="s">
+        <v>266</v>
+      </c>
+      <c r="D388" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="389" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B389">
+        <v>9928229</v>
+      </c>
+      <c r="C389" t="s">
+        <v>266</v>
+      </c>
+      <c r="D389" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="390" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B390">
+        <v>9943073</v>
+      </c>
+      <c r="C390" t="s">
+        <v>266</v>
+      </c>
+      <c r="D390" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="391" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B391">
+        <v>9943085</v>
+      </c>
+      <c r="C391" t="s">
+        <v>266</v>
+      </c>
+      <c r="D391" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="392" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B392">
+        <v>9943097</v>
+      </c>
+      <c r="C392" t="s">
+        <v>266</v>
+      </c>
+      <c r="D392" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="393" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B393">
+        <v>9966116</v>
+      </c>
+      <c r="C393" t="s">
+        <v>266</v>
+      </c>
+      <c r="D393" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="394" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B394">
+        <v>9948748</v>
+      </c>
+      <c r="C394" t="s">
+        <v>266</v>
+      </c>
+      <c r="D394" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="395" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B395">
+        <v>9944546</v>
+      </c>
+      <c r="C395" t="s">
+        <v>266</v>
+      </c>
+      <c r="D395" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="396" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B396">
+        <v>9948750</v>
+      </c>
+      <c r="C396" t="s">
+        <v>266</v>
+      </c>
+      <c r="D396" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="397" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B397">
+        <v>9948774</v>
+      </c>
+      <c r="C397" t="s">
+        <v>266</v>
+      </c>
+      <c r="D397" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="398" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B398">
+        <v>9948815</v>
+      </c>
+      <c r="C398" t="s">
+        <v>266</v>
+      </c>
+      <c r="D398" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="399" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B399">
+        <v>9948762</v>
+      </c>
+      <c r="C399" t="s">
+        <v>266</v>
+      </c>
+      <c r="D399" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="400" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B400">
+        <v>9948786</v>
+      </c>
+      <c r="C400" t="s">
+        <v>266</v>
+      </c>
+      <c r="D400" t="s">
+        <v>265</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
"Equinox and Aegir class added"
</commit_message>
<xml_diff>
--- a/trackedvessels.xlsx
+++ b/trackedvessels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/Vesseltimeline/VesselTimeline_dataGet-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="171" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2179B39-E900-4B53-8185-586A8EA905C7}"/>
+  <xr:revisionPtr revIDLastSave="220" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ABA8DB3-3914-4329-B980-35FB1637F451}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="0" windowWidth="25800" windowHeight="13780" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
+    <workbookView xWindow="25510" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1192" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="459">
   <si>
     <t>Santa Rosa</t>
   </si>
@@ -1350,6 +1350,69 @@
   </si>
   <si>
     <t>Maersk 171</t>
+  </si>
+  <si>
+    <t>MM868</t>
+  </si>
+  <si>
+    <t>Aegir Class</t>
+  </si>
+  <si>
+    <t>Equinox Class</t>
+  </si>
+  <si>
+    <t>Berlin Mærsk</t>
+  </si>
+  <si>
+    <t>Beijing Mærsk</t>
+  </si>
+  <si>
+    <t>Bangkok Mærsk</t>
+  </si>
+  <si>
+    <t>Brisbane Mærsk</t>
+  </si>
+  <si>
+    <t>Brussels Mærsk</t>
+  </si>
+  <si>
+    <t>Barcelona Mærsk</t>
+  </si>
+  <si>
+    <t>Ane Mærsk</t>
+  </si>
+  <si>
+    <t>Astrid Mærsk</t>
+  </si>
+  <si>
+    <t>Antonia Mærsk</t>
+  </si>
+  <si>
+    <t>Alette Mærsk</t>
+  </si>
+  <si>
+    <t>Alexandra Mærsk</t>
+  </si>
+  <si>
+    <t>Angelica Mærsk</t>
+  </si>
+  <si>
+    <t>A. P. Møller</t>
+  </si>
+  <si>
+    <t>Adrian Maersk</t>
+  </si>
+  <si>
+    <t>Albert Maersk</t>
+  </si>
+  <si>
+    <t>Alva Maersk</t>
+  </si>
+  <si>
+    <t>Arthur Maersk</t>
+  </si>
+  <si>
+    <t>Axel Maersk</t>
   </si>
 </sst>
 </file>
@@ -1707,10 +1770,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A49309-98C8-6143-85DD-C6C0E46E1D27}">
-  <dimension ref="A1:D397"/>
+  <dimension ref="A1:D415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A372" workbookViewId="0">
-      <selection activeCell="F388" sqref="F388"/>
+    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
+      <selection activeCell="F404" sqref="F404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7278,6 +7341,258 @@
         <v>265</v>
       </c>
     </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A398" t="s">
+        <v>441</v>
+      </c>
+      <c r="B398">
+        <v>9984560</v>
+      </c>
+      <c r="C398" t="s">
+        <v>439</v>
+      </c>
+      <c r="D398" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A399" t="s">
+        <v>442</v>
+      </c>
+      <c r="B399">
+        <v>9984572</v>
+      </c>
+      <c r="C399" t="s">
+        <v>439</v>
+      </c>
+      <c r="D399" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A400" t="s">
+        <v>443</v>
+      </c>
+      <c r="B400">
+        <v>9984584</v>
+      </c>
+      <c r="C400" t="s">
+        <v>439</v>
+      </c>
+      <c r="D400" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A401" t="s">
+        <v>444</v>
+      </c>
+      <c r="B401">
+        <v>9984596</v>
+      </c>
+      <c r="C401" t="s">
+        <v>439</v>
+      </c>
+      <c r="D401" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A402" t="s">
+        <v>445</v>
+      </c>
+      <c r="B402">
+        <v>9984601</v>
+      </c>
+      <c r="C402" t="s">
+        <v>439</v>
+      </c>
+      <c r="D402" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A403" t="s">
+        <v>446</v>
+      </c>
+      <c r="B403">
+        <v>9984613</v>
+      </c>
+      <c r="C403" t="s">
+        <v>439</v>
+      </c>
+      <c r="D403" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A404" t="s">
+        <v>447</v>
+      </c>
+      <c r="B404">
+        <v>9948748</v>
+      </c>
+      <c r="C404" t="s">
+        <v>440</v>
+      </c>
+      <c r="D404" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A405" t="s">
+        <v>448</v>
+      </c>
+      <c r="B405">
+        <v>9948750</v>
+      </c>
+      <c r="C405" t="s">
+        <v>440</v>
+      </c>
+      <c r="D405" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A406" t="s">
+        <v>449</v>
+      </c>
+      <c r="B406">
+        <v>9948762</v>
+      </c>
+      <c r="C406" t="s">
+        <v>440</v>
+      </c>
+      <c r="D406" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A407" t="s">
+        <v>450</v>
+      </c>
+      <c r="B407">
+        <v>9948774</v>
+      </c>
+      <c r="C407" t="s">
+        <v>440</v>
+      </c>
+      <c r="D407" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A408" t="s">
+        <v>451</v>
+      </c>
+      <c r="B408">
+        <v>9948786</v>
+      </c>
+      <c r="C408" t="s">
+        <v>440</v>
+      </c>
+      <c r="D408" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="409" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A409" t="s">
+        <v>452</v>
+      </c>
+      <c r="B409">
+        <v>9948798</v>
+      </c>
+      <c r="C409" t="s">
+        <v>440</v>
+      </c>
+      <c r="D409" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="410" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A410" t="s">
+        <v>453</v>
+      </c>
+      <c r="B410">
+        <v>9948803</v>
+      </c>
+      <c r="C410" t="s">
+        <v>440</v>
+      </c>
+      <c r="D410" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="411" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A411" t="s">
+        <v>454</v>
+      </c>
+      <c r="B411">
+        <v>9948815</v>
+      </c>
+      <c r="C411" t="s">
+        <v>440</v>
+      </c>
+      <c r="D411" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="412" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A412" t="s">
+        <v>455</v>
+      </c>
+      <c r="B412">
+        <v>9961805</v>
+      </c>
+      <c r="C412" t="s">
+        <v>440</v>
+      </c>
+      <c r="D412" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="413" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A413" t="s">
+        <v>456</v>
+      </c>
+      <c r="B413">
+        <v>9961817</v>
+      </c>
+      <c r="C413" t="s">
+        <v>440</v>
+      </c>
+      <c r="D413" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="414" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A414" t="s">
+        <v>457</v>
+      </c>
+      <c r="B414">
+        <v>9961829</v>
+      </c>
+      <c r="C414" t="s">
+        <v>440</v>
+      </c>
+      <c r="D414" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="415" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A415" t="s">
+        <v>458</v>
+      </c>
+      <c r="B415">
+        <v>9961831</v>
+      </c>
+      <c r="C415" t="s">
+        <v>440</v>
+      </c>
+      <c r="D415" t="s">
+        <v>438</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added Aegir and Equinox class
</commit_message>
<xml_diff>
--- a/trackedvessels.xlsx
+++ b/trackedvessels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/Vesseltimeline/VesselTimeline_dataGet-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="220" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ABA8DB3-3914-4329-B980-35FB1637F451}"/>
+  <xr:revisionPtr revIDLastSave="238" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFA4BA6D-66E6-48A2-83C5-14F083CD2894}"/>
   <bookViews>
     <workbookView xWindow="25510" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
   </bookViews>
@@ -1355,12 +1355,6 @@
     <t>MM868</t>
   </si>
   <si>
-    <t>Aegir Class</t>
-  </si>
-  <si>
-    <t>Equinox Class</t>
-  </si>
-  <si>
     <t>Berlin Mærsk</t>
   </si>
   <si>
@@ -1413,6 +1407,12 @@
   </si>
   <si>
     <t>Axel Maersk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aegir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equinox </t>
   </si>
 </sst>
 </file>
@@ -1772,8 +1772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A49309-98C8-6143-85DD-C6C0E46E1D27}">
   <dimension ref="A1:D415"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
-      <selection activeCell="F404" sqref="F404"/>
+    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="E406" sqref="E406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7343,13 +7343,13 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B398">
         <v>9984560</v>
       </c>
       <c r="C398" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="D398" t="s">
         <v>438</v>
@@ -7357,13 +7357,13 @@
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B399">
         <v>9984572</v>
       </c>
       <c r="C399" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="D399" t="s">
         <v>438</v>
@@ -7371,13 +7371,13 @@
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B400">
         <v>9984584</v>
       </c>
       <c r="C400" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="D400" t="s">
         <v>438</v>
@@ -7385,13 +7385,13 @@
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B401">
         <v>9984596</v>
       </c>
       <c r="C401" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="D401" t="s">
         <v>438</v>
@@ -7399,13 +7399,13 @@
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B402">
         <v>9984601</v>
       </c>
       <c r="C402" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="D402" t="s">
         <v>438</v>
@@ -7413,13 +7413,13 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B403">
         <v>9984613</v>
       </c>
       <c r="C403" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="D403" t="s">
         <v>438</v>
@@ -7427,13 +7427,13 @@
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B404">
         <v>9948748</v>
       </c>
       <c r="C404" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D404" t="s">
         <v>438</v>
@@ -7441,13 +7441,13 @@
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B405">
         <v>9948750</v>
       </c>
       <c r="C405" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D405" t="s">
         <v>438</v>
@@ -7455,13 +7455,13 @@
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B406">
         <v>9948762</v>
       </c>
       <c r="C406" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D406" t="s">
         <v>438</v>
@@ -7469,13 +7469,13 @@
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B407">
         <v>9948774</v>
       </c>
       <c r="C407" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D407" t="s">
         <v>438</v>
@@ -7483,13 +7483,13 @@
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B408">
         <v>9948786</v>
       </c>
       <c r="C408" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D408" t="s">
         <v>438</v>
@@ -7497,13 +7497,13 @@
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B409">
         <v>9948798</v>
       </c>
       <c r="C409" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D409" t="s">
         <v>438</v>
@@ -7511,13 +7511,13 @@
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B410">
         <v>9948803</v>
       </c>
       <c r="C410" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D410" t="s">
         <v>438</v>
@@ -7525,13 +7525,13 @@
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B411">
         <v>9948815</v>
       </c>
       <c r="C411" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D411" t="s">
         <v>438</v>
@@ -7539,13 +7539,13 @@
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B412">
         <v>9961805</v>
       </c>
       <c r="C412" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D412" t="s">
         <v>438</v>
@@ -7553,13 +7553,13 @@
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B413">
         <v>9961817</v>
       </c>
       <c r="C413" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D413" t="s">
         <v>438</v>
@@ -7567,13 +7567,13 @@
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B414">
         <v>9961829</v>
       </c>
       <c r="C414" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D414" t="s">
         <v>438</v>
@@ -7581,13 +7581,13 @@
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B415">
         <v>9961831</v>
       </c>
       <c r="C415" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="D415" t="s">
         <v>438</v>

</xml_diff>

<commit_message>
added Aegir and Equinox classes
</commit_message>
<xml_diff>
--- a/trackedvessels.xlsx
+++ b/trackedvessels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://marinefluid-my.sharepoint.com/personal/anders_busk_marinefluid_dk/Documents/Desktop/Vesseltimeline/VesselTimeline_dataGet-main/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="238" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFA4BA6D-66E6-48A2-83C5-14F083CD2894}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="8_{040B8FFE-810C-44D2-BC43-6E99EF4554CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9308C3E6-ACEA-4548-B330-255D699DA82E}"/>
   <bookViews>
     <workbookView xWindow="25510" yWindow="0" windowWidth="25780" windowHeight="13770" xr2:uid="{EAC07ED0-C752-7C43-A5B0-616708F842E7}"/>
   </bookViews>
@@ -1352,67 +1352,67 @@
     <t>Maersk 171</t>
   </si>
   <si>
-    <t>MM868</t>
-  </si>
-  <si>
-    <t>Berlin Mærsk</t>
-  </si>
-  <si>
-    <t>Beijing Mærsk</t>
-  </si>
-  <si>
-    <t>Bangkok Mærsk</t>
-  </si>
-  <si>
-    <t>Brisbane Mærsk</t>
-  </si>
-  <si>
-    <t>Brussels Mærsk</t>
-  </si>
-  <si>
-    <t>Barcelona Mærsk</t>
-  </si>
-  <si>
-    <t>Ane Mærsk</t>
-  </si>
-  <si>
-    <t>Astrid Mærsk</t>
-  </si>
-  <si>
-    <t>Antonia Mærsk</t>
-  </si>
-  <si>
-    <t>Alette Mærsk</t>
-  </si>
-  <si>
-    <t>Alexandra Mærsk</t>
-  </si>
-  <si>
-    <t>Angelica Mærsk</t>
-  </si>
-  <si>
-    <t>A. P. Møller</t>
-  </si>
-  <si>
-    <t>Adrian Maersk</t>
-  </si>
-  <si>
-    <t>Albert Maersk</t>
-  </si>
-  <si>
-    <t>Alva Maersk</t>
-  </si>
-  <si>
-    <t>Arthur Maersk</t>
-  </si>
-  <si>
-    <t>Axel Maersk</t>
-  </si>
-  <si>
     <t xml:space="preserve">Aegir </t>
   </si>
   <si>
     <t xml:space="preserve">Equinox </t>
+  </si>
+  <si>
+    <t>Maersk 172</t>
+  </si>
+  <si>
+    <t>Maersk 173</t>
+  </si>
+  <si>
+    <t>Maersk 174</t>
+  </si>
+  <si>
+    <t>Maersk 175</t>
+  </si>
+  <si>
+    <t>Maersk 176</t>
+  </si>
+  <si>
+    <t>Maersk 177</t>
+  </si>
+  <si>
+    <t>Maersk 178</t>
+  </si>
+  <si>
+    <t>Maersk 179</t>
+  </si>
+  <si>
+    <t>Maersk 180</t>
+  </si>
+  <si>
+    <t>Maersk 181</t>
+  </si>
+  <si>
+    <t>Maersk 182</t>
+  </si>
+  <si>
+    <t>Maersk 183</t>
+  </si>
+  <si>
+    <t>Maersk 184</t>
+  </si>
+  <si>
+    <t>Maersk 185</t>
+  </si>
+  <si>
+    <t>Maersk 186</t>
+  </si>
+  <si>
+    <t>Maersk 187</t>
+  </si>
+  <si>
+    <t>Maersk 188</t>
+  </si>
+  <si>
+    <t>Maersk 189</t>
+  </si>
+  <si>
+    <t>M868</t>
   </si>
 </sst>
 </file>
@@ -1773,7 +1773,7 @@
   <dimension ref="A1:D415"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
-      <selection activeCell="E406" sqref="E406"/>
+      <selection activeCell="F411" sqref="F411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7343,254 +7343,254 @@
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B398">
         <v>9984560</v>
       </c>
       <c r="C398" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="D398" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B399">
         <v>9984572</v>
       </c>
       <c r="C399" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="D399" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B400">
         <v>9984584</v>
       </c>
       <c r="C400" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="D400" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B401">
         <v>9984596</v>
       </c>
       <c r="C401" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="D401" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B402">
         <v>9984601</v>
       </c>
       <c r="C402" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="D402" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="B403">
         <v>9984613</v>
       </c>
       <c r="C403" t="s">
-        <v>457</v>
+        <v>438</v>
       </c>
       <c r="D403" t="s">
-        <v>438</v>
+        <v>458</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B404">
         <v>9948748</v>
       </c>
       <c r="C404" t="s">
+        <v>439</v>
+      </c>
+      <c r="D404" t="s">
         <v>458</v>
-      </c>
-      <c r="D404" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="405" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B405">
         <v>9948750</v>
       </c>
       <c r="C405" t="s">
+        <v>439</v>
+      </c>
+      <c r="D405" t="s">
         <v>458</v>
-      </c>
-      <c r="D405" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B406">
         <v>9948762</v>
       </c>
       <c r="C406" t="s">
+        <v>439</v>
+      </c>
+      <c r="D406" t="s">
         <v>458</v>
-      </c>
-      <c r="D406" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="B407">
         <v>9948774</v>
       </c>
       <c r="C407" t="s">
+        <v>439</v>
+      </c>
+      <c r="D407" t="s">
         <v>458</v>
-      </c>
-      <c r="D407" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="B408">
         <v>9948786</v>
       </c>
       <c r="C408" t="s">
+        <v>439</v>
+      </c>
+      <c r="D408" t="s">
         <v>458</v>
-      </c>
-      <c r="D408" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B409">
         <v>9948798</v>
       </c>
       <c r="C409" t="s">
+        <v>439</v>
+      </c>
+      <c r="D409" t="s">
         <v>458</v>
-      </c>
-      <c r="D409" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B410">
         <v>9948803</v>
       </c>
       <c r="C410" t="s">
+        <v>439</v>
+      </c>
+      <c r="D410" t="s">
         <v>458</v>
-      </c>
-      <c r="D410" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B411">
         <v>9948815</v>
       </c>
       <c r="C411" t="s">
+        <v>439</v>
+      </c>
+      <c r="D411" t="s">
         <v>458</v>
-      </c>
-      <c r="D411" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="412" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B412">
         <v>9961805</v>
       </c>
       <c r="C412" t="s">
+        <v>439</v>
+      </c>
+      <c r="D412" t="s">
         <v>458</v>
-      </c>
-      <c r="D412" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B413">
         <v>9961817</v>
       </c>
       <c r="C413" t="s">
+        <v>439</v>
+      </c>
+      <c r="D413" t="s">
         <v>458</v>
-      </c>
-      <c r="D413" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="B414">
         <v>9961829</v>
       </c>
       <c r="C414" t="s">
+        <v>439</v>
+      </c>
+      <c r="D414" t="s">
         <v>458</v>
-      </c>
-      <c r="D414" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="415" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B415">
         <v>9961831</v>
       </c>
       <c r="C415" t="s">
+        <v>439</v>
+      </c>
+      <c r="D415" t="s">
         <v>458</v>
-      </c>
-      <c r="D415" t="s">
-        <v>438</v>
       </c>
     </row>
   </sheetData>

</xml_diff>